<commit_message>
Corrected Input files for 2 test cases COTC022
</commit_message>
<xml_diff>
--- a/InputFiles/ICDC/TC04_Canine_Study-COTC022_Breed-AmericanStaffordshireTerrier.xlsx
+++ b/InputFiles/ICDC/TC04_Canine_Study-COTC022_Breed-AmericanStaffordshireTerrier.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\ICDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08520BE-DA0B-4F91-B31A-94E6FC07FDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF3F38B-E2FD-4702-82EA-266D5357D407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -101,11 +101,33 @@
 limit 100</t>
   </si>
   <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+  WHERE s.clinical_study_designation IN ['COTC022'] and demo.breed IN ['American Staffordshire Terrier']
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>TC04_Canine_Study-COTC022_Breed-AmericanStaffordshireTerrier_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC04_Canine_Study-COTC022_Breed-AmericanStaffordshireTerrier_WebData.xlsx</t>
+  </si>
+  <si>
     <t>MATCH (f:file)--&gt;(parent)
 MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
 MATCH (diag:diagnosis)--&gt;(c)
 WHERE demo.breed IN ['American Staffordshire Terrier']
-OPTIONAL MATCH (s:study)&lt;--(c)
+MATCH (s:study)&lt;--(c)
 WHERE s.clinical_study_designation IN ['COTC022']
 OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
 WITH
@@ -139,8 +161,8 @@
     <t>MATCH (f:file)--&gt;(s:study)
 WHERE s.clinical_study_designation IN ['COTC022']
 MATCH (s)&lt;--(c:case)&lt;--(diag:diagnosis)
+MATCH (c)&lt;--(demo:demographic)
 WHERE demo.breed IN ['American Staffordshire Terrier']
-MATCH (c)&lt;--(demo:demographic)
 WITH
         DISTINCT f, c, demo, diag, s,
         ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
@@ -163,28 +185,6 @@
   coalesce(s.clinical_study_designation,'') AS `Study Code`
   order by 'File Name' asc
   limit 100</t>
-  </si>
-  <si>
-    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
-OPTIONAL MATCH (f:file)-[*]-&gt;(c)
-OPTIONAL MATCH (sf:file)--&gt;(s)
-WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
-  WHERE s.clinical_study_designation IN ['COTC022'] and demo.breed IN ['American Staffordshire Terrier']
-RETURN  
-    count(distinct p) AS Programs,
-    count(distinct s) AS Studies,
-    count(distinct c) AS Cases,
-    count(distinct samp) AS Samples,
-    count(distinct f) AS `Case Files`,
-    count(distinct sf) AS `Study Files`</t>
-  </si>
-  <si>
-    <t>TC04_Canine_Study-COTC022_Breed-AmericanStaffordshireTerrier_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC04_Canine_Study-COTC022_Breed-AmericanStaffordshireTerrier_WebData.xlsx</t>
   </si>
 </sst>
 </file>
@@ -258,9 +258,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -298,7 +298,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -404,7 +404,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -546,7 +546,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -594,13 +594,13 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="261" x14ac:dyDescent="0.35">
@@ -611,13 +611,13 @@
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
@@ -625,16 +625,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="391.5" x14ac:dyDescent="0.35">
@@ -642,16 +642,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>